<commit_message>
EPBDS-8931 REST services uses incorrect media type for simple types of data (text/plain) EPBDS-9033 Improve HttpClient in ITEST to simplify comparing JSON structure
</commit_message>
<xml_diff>
--- a/ITEST/itest.smoke/openl-repository/deployments/simple/simple.xlsx
+++ b/ITEST/itest.smoke/openl-repository/deployments/simple/simple.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\openL\ITEST\itest.smoke\openl-repository\deployments\simple\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A4571C-A91E-475A-99C9-552E84ED442F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="19635" windowHeight="8190"/>
+    <workbookView xWindow="0" yWindow="180" windowWidth="28800" windowHeight="7830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="5" r:id="rId1"/>
@@ -19,13 +25,7 @@
     <t>return num*2;</t>
   </si>
   <si>
-    <t>Method String ping()</t>
-  </si>
-  <si>
     <t>return "Pong!";</t>
-  </si>
-  <si>
-    <t>Method Integer twice (Integer num)</t>
   </si>
   <si>
     <t>Method Integer mul (int x, Integer y)</t>
@@ -33,11 +33,17 @@
   <si>
     <t>return x*y;</t>
   </si>
+  <si>
+    <t>Method Integer twice (Integer num)</t>
+  </si>
+  <si>
+    <t>Method String ping()</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -68,7 +74,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -144,14 +150,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -189,9 +198,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -224,9 +233,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -259,9 +285,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -434,11 +477,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -448,7 +491,7 @@
   <sheetData>
     <row r="3" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.2">
@@ -458,22 +501,22 @@
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>